<commit_message>
feat: import baby localize
</commit_message>
<xml_diff>
--- a/public/static/template/import_baby_en.xlsx
+++ b/public/static/template/import_baby_en.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="41">
   <si>
     <t>Baby ID</t>
   </si>
@@ -243,26 +243,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Monaco"/>
-      </rPr>
-      <t xml:space="preserve">1.Required
-</t>
-    </r>
-    <r>
-      <rPr>
-        <strike val="1"/>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Monaco"/>
-      </rPr>
-      <t>2.Format：</t>
-    </r>
-  </si>
-  <si>
     <t>1.Required</t>
   </si>
   <si>
@@ -284,7 +264,7 @@
         <color indexed="8"/>
         <rFont val="Monaco"/>
       </rPr>
-      <t>2.Relatives Options: Monther/Father/Grandmother</t>
+      <t>2.Relatives Options: Mother/Father/Grandmother</t>
     </r>
     <r>
       <rPr>
@@ -374,15 +354,6 @@
       <t xml:space="preserve">1.Required
 </t>
     </r>
-    <r>
-      <rPr>
-        <strike val="1"/>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Monaco"/>
-      </rPr>
-      <t>2.Validate:</t>
-    </r>
   </si>
   <si>
     <t>Wechat</t>
@@ -422,10 +393,10 @@
       <name val="Monaco"/>
     </font>
     <font>
-      <strike val="1"/>
-      <sz val="11"/>
-      <color indexed="8"/>
-      <name val="Monaco"/>
+      <b val="1"/>
+      <sz val="16"/>
+      <color indexed="13"/>
+      <name val="Helvetica"/>
     </font>
   </fonts>
   <fills count="4">
@@ -477,7 +448,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -517,6 +488,15 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -541,6 +521,7 @@
       <rgbColor rgb="ffaaaaaa"/>
       <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffcccccc"/>
+      <rgbColor rgb="ff4a4a4a"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -1725,23 +1706,23 @@
         <v>36</v>
       </c>
       <c r="J2" t="s" s="6">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K2" s="8"/>
       <c r="L2" t="s" s="7">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M2" t="s" s="6">
         <v>30</v>
       </c>
       <c r="N2" t="s" s="6">
+        <v>38</v>
+      </c>
+      <c r="O2" t="s" s="6">
         <v>39</v>
       </c>
-      <c r="O2" t="s" s="6">
+      <c r="P2" t="s" s="7">
         <v>40</v>
-      </c>
-      <c r="P2" t="s" s="7">
-        <v>41</v>
       </c>
       <c r="Q2" s="8"/>
       <c r="R2" s="8"/>
@@ -1769,9 +1750,9 @@
       <c r="I3" s="12"/>
       <c r="J3" s="12"/>
       <c r="K3" s="12"/>
-      <c r="L3" s="9"/>
-      <c r="M3" s="11"/>
-      <c r="N3" s="13"/>
+      <c r="L3" s="13"/>
+      <c r="M3" s="14"/>
+      <c r="N3" s="15"/>
       <c r="O3" s="11"/>
       <c r="P3" s="12"/>
       <c r="Q3" s="12"/>
@@ -1789,21 +1770,21 @@
       <c r="AC3" s="12"/>
     </row>
     <row r="4" ht="16" customHeight="1">
-      <c r="A4" s="12"/>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
+      <c r="A4" s="9"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
       <c r="E4" s="11"/>
       <c r="F4" s="11"/>
       <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
+      <c r="H4" s="8"/>
       <c r="I4" s="12"/>
       <c r="J4" s="12"/>
       <c r="K4" s="12"/>
-      <c r="L4" s="12"/>
-      <c r="M4" s="12"/>
-      <c r="N4" s="13"/>
-      <c r="O4" s="12"/>
+      <c r="L4" s="13"/>
+      <c r="M4" s="14"/>
+      <c r="N4" s="15"/>
+      <c r="O4" s="11"/>
       <c r="P4" s="12"/>
       <c r="Q4" s="12"/>
       <c r="R4" s="12"/>
@@ -1833,7 +1814,7 @@
       <c r="K5" s="12"/>
       <c r="L5" s="12"/>
       <c r="M5" s="12"/>
-      <c r="N5" s="13"/>
+      <c r="N5" s="16"/>
       <c r="O5" s="12"/>
       <c r="P5" s="12"/>
       <c r="Q5" s="12"/>
@@ -1864,7 +1845,7 @@
       <c r="K6" s="12"/>
       <c r="L6" s="12"/>
       <c r="M6" s="12"/>
-      <c r="N6" s="13"/>
+      <c r="N6" s="16"/>
       <c r="O6" s="12"/>
       <c r="P6" s="12"/>
       <c r="Q6" s="12"/>
@@ -1895,7 +1876,7 @@
       <c r="K7" s="12"/>
       <c r="L7" s="12"/>
       <c r="M7" s="12"/>
-      <c r="N7" s="13"/>
+      <c r="N7" s="16"/>
       <c r="O7" s="12"/>
       <c r="P7" s="12"/>
       <c r="Q7" s="12"/>
@@ -1926,7 +1907,7 @@
       <c r="K8" s="12"/>
       <c r="L8" s="12"/>
       <c r="M8" s="12"/>
-      <c r="N8" s="13"/>
+      <c r="N8" s="16"/>
       <c r="O8" s="12"/>
       <c r="P8" s="12"/>
       <c r="Q8" s="12"/>
@@ -1957,7 +1938,7 @@
       <c r="K9" s="12"/>
       <c r="L9" s="12"/>
       <c r="M9" s="12"/>
-      <c r="N9" s="13"/>
+      <c r="N9" s="16"/>
       <c r="O9" s="12"/>
       <c r="P9" s="12"/>
       <c r="Q9" s="12"/>
@@ -1988,7 +1969,7 @@
       <c r="K10" s="12"/>
       <c r="L10" s="12"/>
       <c r="M10" s="12"/>
-      <c r="N10" s="13"/>
+      <c r="N10" s="16"/>
       <c r="O10" s="12"/>
       <c r="P10" s="12"/>
       <c r="Q10" s="12"/>
@@ -2019,7 +2000,7 @@
       <c r="K11" s="12"/>
       <c r="L11" s="12"/>
       <c r="M11" s="12"/>
-      <c r="N11" s="13"/>
+      <c r="N11" s="16"/>
       <c r="O11" s="12"/>
       <c r="P11" s="12"/>
       <c r="Q11" s="12"/>
@@ -2050,7 +2031,7 @@
       <c r="K12" s="12"/>
       <c r="L12" s="12"/>
       <c r="M12" s="12"/>
-      <c r="N12" s="13"/>
+      <c r="N12" s="16"/>
       <c r="O12" s="12"/>
       <c r="P12" s="12"/>
       <c r="Q12" s="12"/>
@@ -2081,7 +2062,7 @@
       <c r="K13" s="12"/>
       <c r="L13" s="12"/>
       <c r="M13" s="12"/>
-      <c r="N13" s="13"/>
+      <c r="N13" s="16"/>
       <c r="O13" s="12"/>
       <c r="P13" s="12"/>
       <c r="Q13" s="12"/>
@@ -2112,7 +2093,7 @@
       <c r="K14" s="12"/>
       <c r="L14" s="12"/>
       <c r="M14" s="12"/>
-      <c r="N14" s="13"/>
+      <c r="N14" s="16"/>
       <c r="O14" s="12"/>
       <c r="P14" s="12"/>
       <c r="Q14" s="12"/>
@@ -2143,7 +2124,7 @@
       <c r="K15" s="12"/>
       <c r="L15" s="12"/>
       <c r="M15" s="12"/>
-      <c r="N15" s="13"/>
+      <c r="N15" s="16"/>
       <c r="O15" s="12"/>
       <c r="P15" s="12"/>
       <c r="Q15" s="12"/>
@@ -2174,7 +2155,7 @@
       <c r="K16" s="12"/>
       <c r="L16" s="12"/>
       <c r="M16" s="12"/>
-      <c r="N16" s="13"/>
+      <c r="N16" s="16"/>
       <c r="O16" s="12"/>
       <c r="P16" s="12"/>
       <c r="Q16" s="12"/>
@@ -2205,7 +2186,7 @@
       <c r="K17" s="12"/>
       <c r="L17" s="12"/>
       <c r="M17" s="12"/>
-      <c r="N17" s="13"/>
+      <c r="N17" s="16"/>
       <c r="O17" s="12"/>
       <c r="P17" s="12"/>
       <c r="Q17" s="12"/>
@@ -2236,7 +2217,7 @@
       <c r="K18" s="12"/>
       <c r="L18" s="12"/>
       <c r="M18" s="12"/>
-      <c r="N18" s="13"/>
+      <c r="N18" s="16"/>
       <c r="O18" s="12"/>
       <c r="P18" s="12"/>
       <c r="Q18" s="12"/>
@@ -2267,7 +2248,7 @@
       <c r="K19" s="12"/>
       <c r="L19" s="12"/>
       <c r="M19" s="12"/>
-      <c r="N19" s="13"/>
+      <c r="N19" s="16"/>
       <c r="O19" s="12"/>
       <c r="P19" s="12"/>
       <c r="Q19" s="12"/>
@@ -2298,7 +2279,7 @@
       <c r="K20" s="12"/>
       <c r="L20" s="12"/>
       <c r="M20" s="12"/>
-      <c r="N20" s="13"/>
+      <c r="N20" s="16"/>
       <c r="O20" s="12"/>
       <c r="P20" s="12"/>
       <c r="Q20" s="12"/>
@@ -2329,7 +2310,7 @@
       <c r="K21" s="12"/>
       <c r="L21" s="12"/>
       <c r="M21" s="12"/>
-      <c r="N21" s="13"/>
+      <c r="N21" s="16"/>
       <c r="O21" s="12"/>
       <c r="P21" s="12"/>
       <c r="Q21" s="12"/>
@@ -2360,7 +2341,7 @@
       <c r="K22" s="12"/>
       <c r="L22" s="12"/>
       <c r="M22" s="12"/>
-      <c r="N22" s="13"/>
+      <c r="N22" s="16"/>
       <c r="O22" s="12"/>
       <c r="P22" s="12"/>
       <c r="Q22" s="12"/>
@@ -2391,7 +2372,7 @@
       <c r="K23" s="12"/>
       <c r="L23" s="12"/>
       <c r="M23" s="12"/>
-      <c r="N23" s="13"/>
+      <c r="N23" s="16"/>
       <c r="O23" s="12"/>
       <c r="P23" s="12"/>
       <c r="Q23" s="12"/>
@@ -2422,7 +2403,7 @@
       <c r="K24" s="12"/>
       <c r="L24" s="12"/>
       <c r="M24" s="12"/>
-      <c r="N24" s="13"/>
+      <c r="N24" s="16"/>
       <c r="O24" s="12"/>
       <c r="P24" s="12"/>
       <c r="Q24" s="12"/>
@@ -2453,7 +2434,7 @@
       <c r="K25" s="12"/>
       <c r="L25" s="12"/>
       <c r="M25" s="12"/>
-      <c r="N25" s="13"/>
+      <c r="N25" s="16"/>
       <c r="O25" s="12"/>
       <c r="P25" s="12"/>
       <c r="Q25" s="12"/>
@@ -2484,7 +2465,7 @@
       <c r="K26" s="12"/>
       <c r="L26" s="12"/>
       <c r="M26" s="12"/>
-      <c r="N26" s="13"/>
+      <c r="N26" s="16"/>
       <c r="O26" s="12"/>
       <c r="P26" s="12"/>
       <c r="Q26" s="12"/>
@@ -2515,7 +2496,7 @@
       <c r="K27" s="12"/>
       <c r="L27" s="12"/>
       <c r="M27" s="12"/>
-      <c r="N27" s="13"/>
+      <c r="N27" s="16"/>
       <c r="O27" s="12"/>
       <c r="P27" s="12"/>
       <c r="Q27" s="12"/>
@@ -2546,7 +2527,7 @@
       <c r="K28" s="12"/>
       <c r="L28" s="12"/>
       <c r="M28" s="12"/>
-      <c r="N28" s="13"/>
+      <c r="N28" s="16"/>
       <c r="O28" s="12"/>
       <c r="P28" s="12"/>
       <c r="Q28" s="12"/>
@@ -2577,7 +2558,7 @@
       <c r="K29" s="12"/>
       <c r="L29" s="12"/>
       <c r="M29" s="12"/>
-      <c r="N29" s="13"/>
+      <c r="N29" s="16"/>
       <c r="O29" s="12"/>
       <c r="P29" s="12"/>
       <c r="Q29" s="12"/>
@@ -2608,7 +2589,7 @@
       <c r="K30" s="12"/>
       <c r="L30" s="12"/>
       <c r="M30" s="12"/>
-      <c r="N30" s="13"/>
+      <c r="N30" s="16"/>
       <c r="O30" s="12"/>
       <c r="P30" s="12"/>
       <c r="Q30" s="12"/>
@@ -2639,7 +2620,7 @@
       <c r="K31" s="12"/>
       <c r="L31" s="12"/>
       <c r="M31" s="12"/>
-      <c r="N31" s="13"/>
+      <c r="N31" s="16"/>
       <c r="O31" s="12"/>
       <c r="P31" s="12"/>
       <c r="Q31" s="12"/>
@@ -2670,7 +2651,7 @@
       <c r="K32" s="12"/>
       <c r="L32" s="12"/>
       <c r="M32" s="12"/>
-      <c r="N32" s="13"/>
+      <c r="N32" s="16"/>
       <c r="O32" s="12"/>
       <c r="P32" s="12"/>
       <c r="Q32" s="12"/>
@@ -2701,7 +2682,7 @@
       <c r="K33" s="12"/>
       <c r="L33" s="12"/>
       <c r="M33" s="12"/>
-      <c r="N33" s="13"/>
+      <c r="N33" s="16"/>
       <c r="O33" s="12"/>
       <c r="P33" s="12"/>
       <c r="Q33" s="12"/>
@@ -2732,7 +2713,7 @@
       <c r="K34" s="12"/>
       <c r="L34" s="12"/>
       <c r="M34" s="12"/>
-      <c r="N34" s="13"/>
+      <c r="N34" s="16"/>
       <c r="O34" s="12"/>
       <c r="P34" s="12"/>
       <c r="Q34" s="12"/>
@@ -2763,7 +2744,7 @@
       <c r="K35" s="12"/>
       <c r="L35" s="12"/>
       <c r="M35" s="12"/>
-      <c r="N35" s="13"/>
+      <c r="N35" s="16"/>
       <c r="O35" s="12"/>
       <c r="P35" s="12"/>
       <c r="Q35" s="12"/>
@@ -2794,7 +2775,7 @@
       <c r="K36" s="12"/>
       <c r="L36" s="12"/>
       <c r="M36" s="12"/>
-      <c r="N36" s="13"/>
+      <c r="N36" s="16"/>
       <c r="O36" s="12"/>
       <c r="P36" s="12"/>
       <c r="Q36" s="12"/>
@@ -2825,7 +2806,7 @@
       <c r="K37" s="12"/>
       <c r="L37" s="12"/>
       <c r="M37" s="12"/>
-      <c r="N37" s="13"/>
+      <c r="N37" s="16"/>
       <c r="O37" s="12"/>
       <c r="P37" s="12"/>
       <c r="Q37" s="12"/>
@@ -2856,7 +2837,7 @@
       <c r="K38" s="12"/>
       <c r="L38" s="12"/>
       <c r="M38" s="12"/>
-      <c r="N38" s="13"/>
+      <c r="N38" s="16"/>
       <c r="O38" s="12"/>
       <c r="P38" s="12"/>
       <c r="Q38" s="12"/>
@@ -2887,7 +2868,7 @@
       <c r="K39" s="12"/>
       <c r="L39" s="12"/>
       <c r="M39" s="12"/>
-      <c r="N39" s="13"/>
+      <c r="N39" s="16"/>
       <c r="O39" s="12"/>
       <c r="P39" s="12"/>
       <c r="Q39" s="12"/>
@@ -2918,7 +2899,7 @@
       <c r="K40" s="12"/>
       <c r="L40" s="12"/>
       <c r="M40" s="12"/>
-      <c r="N40" s="13"/>
+      <c r="N40" s="16"/>
       <c r="O40" s="12"/>
       <c r="P40" s="12"/>
       <c r="Q40" s="12"/>
@@ -2949,7 +2930,7 @@
       <c r="K41" s="12"/>
       <c r="L41" s="12"/>
       <c r="M41" s="12"/>
-      <c r="N41" s="13"/>
+      <c r="N41" s="16"/>
       <c r="O41" s="12"/>
       <c r="P41" s="12"/>
       <c r="Q41" s="12"/>
@@ -2980,7 +2961,7 @@
       <c r="K42" s="12"/>
       <c r="L42" s="12"/>
       <c r="M42" s="12"/>
-      <c r="N42" s="13"/>
+      <c r="N42" s="16"/>
       <c r="O42" s="12"/>
       <c r="P42" s="12"/>
       <c r="Q42" s="12"/>
@@ -3011,7 +2992,7 @@
       <c r="K43" s="12"/>
       <c r="L43" s="12"/>
       <c r="M43" s="12"/>
-      <c r="N43" s="13"/>
+      <c r="N43" s="16"/>
       <c r="O43" s="12"/>
       <c r="P43" s="12"/>
       <c r="Q43" s="12"/>
@@ -3042,7 +3023,7 @@
       <c r="K44" s="12"/>
       <c r="L44" s="12"/>
       <c r="M44" s="12"/>
-      <c r="N44" s="13"/>
+      <c r="N44" s="16"/>
       <c r="O44" s="12"/>
       <c r="P44" s="12"/>
       <c r="Q44" s="12"/>
@@ -3073,7 +3054,7 @@
       <c r="K45" s="12"/>
       <c r="L45" s="12"/>
       <c r="M45" s="12"/>
-      <c r="N45" s="13"/>
+      <c r="N45" s="16"/>
       <c r="O45" s="12"/>
       <c r="P45" s="12"/>
       <c r="Q45" s="12"/>
@@ -3104,7 +3085,7 @@
       <c r="K46" s="12"/>
       <c r="L46" s="12"/>
       <c r="M46" s="12"/>
-      <c r="N46" s="13"/>
+      <c r="N46" s="16"/>
       <c r="O46" s="12"/>
       <c r="P46" s="12"/>
       <c r="Q46" s="12"/>
@@ -3135,7 +3116,7 @@
       <c r="K47" s="12"/>
       <c r="L47" s="12"/>
       <c r="M47" s="12"/>
-      <c r="N47" s="13"/>
+      <c r="N47" s="16"/>
       <c r="O47" s="12"/>
       <c r="P47" s="12"/>
       <c r="Q47" s="12"/>
@@ -3166,7 +3147,7 @@
       <c r="K48" s="12"/>
       <c r="L48" s="12"/>
       <c r="M48" s="12"/>
-      <c r="N48" s="13"/>
+      <c r="N48" s="16"/>
       <c r="O48" s="12"/>
       <c r="P48" s="12"/>
       <c r="Q48" s="12"/>
@@ -3197,7 +3178,7 @@
       <c r="K49" s="12"/>
       <c r="L49" s="12"/>
       <c r="M49" s="12"/>
-      <c r="N49" s="13"/>
+      <c r="N49" s="16"/>
       <c r="O49" s="12"/>
       <c r="P49" s="12"/>
       <c r="Q49" s="12"/>
@@ -3228,7 +3209,7 @@
       <c r="K50" s="12"/>
       <c r="L50" s="12"/>
       <c r="M50" s="12"/>
-      <c r="N50" s="13"/>
+      <c r="N50" s="16"/>
       <c r="O50" s="12"/>
       <c r="P50" s="12"/>
       <c r="Q50" s="12"/>
@@ -3259,7 +3240,7 @@
       <c r="K51" s="12"/>
       <c r="L51" s="12"/>
       <c r="M51" s="12"/>
-      <c r="N51" s="13"/>
+      <c r="N51" s="16"/>
       <c r="O51" s="12"/>
       <c r="P51" s="12"/>
       <c r="Q51" s="12"/>
@@ -3290,7 +3271,7 @@
       <c r="K52" s="12"/>
       <c r="L52" s="12"/>
       <c r="M52" s="12"/>
-      <c r="N52" s="13"/>
+      <c r="N52" s="16"/>
       <c r="O52" s="12"/>
       <c r="P52" s="12"/>
       <c r="Q52" s="12"/>
@@ -3321,7 +3302,7 @@
       <c r="K53" s="12"/>
       <c r="L53" s="12"/>
       <c r="M53" s="12"/>
-      <c r="N53" s="13"/>
+      <c r="N53" s="16"/>
       <c r="O53" s="12"/>
       <c r="P53" s="12"/>
       <c r="Q53" s="12"/>
@@ -3352,7 +3333,7 @@
       <c r="K54" s="12"/>
       <c r="L54" s="12"/>
       <c r="M54" s="12"/>
-      <c r="N54" s="13"/>
+      <c r="N54" s="16"/>
       <c r="O54" s="12"/>
       <c r="P54" s="12"/>
       <c r="Q54" s="12"/>
@@ -3383,7 +3364,7 @@
       <c r="K55" s="12"/>
       <c r="L55" s="12"/>
       <c r="M55" s="12"/>
-      <c r="N55" s="13"/>
+      <c r="N55" s="16"/>
       <c r="O55" s="12"/>
       <c r="P55" s="12"/>
       <c r="Q55" s="12"/>
@@ -3414,7 +3395,7 @@
       <c r="K56" s="12"/>
       <c r="L56" s="12"/>
       <c r="M56" s="12"/>
-      <c r="N56" s="13"/>
+      <c r="N56" s="16"/>
       <c r="O56" s="12"/>
       <c r="P56" s="12"/>
       <c r="Q56" s="12"/>
@@ -3445,7 +3426,7 @@
       <c r="K57" s="12"/>
       <c r="L57" s="12"/>
       <c r="M57" s="12"/>
-      <c r="N57" s="13"/>
+      <c r="N57" s="16"/>
       <c r="O57" s="12"/>
       <c r="P57" s="12"/>
       <c r="Q57" s="12"/>
@@ -3476,7 +3457,7 @@
       <c r="K58" s="12"/>
       <c r="L58" s="12"/>
       <c r="M58" s="12"/>
-      <c r="N58" s="13"/>
+      <c r="N58" s="16"/>
       <c r="O58" s="12"/>
       <c r="P58" s="12"/>
       <c r="Q58" s="12"/>
@@ -3507,7 +3488,7 @@
       <c r="K59" s="12"/>
       <c r="L59" s="12"/>
       <c r="M59" s="12"/>
-      <c r="N59" s="13"/>
+      <c r="N59" s="16"/>
       <c r="O59" s="12"/>
       <c r="P59" s="12"/>
       <c r="Q59" s="12"/>
@@ -3538,7 +3519,7 @@
       <c r="K60" s="12"/>
       <c r="L60" s="12"/>
       <c r="M60" s="12"/>
-      <c r="N60" s="13"/>
+      <c r="N60" s="16"/>
       <c r="O60" s="12"/>
       <c r="P60" s="12"/>
       <c r="Q60" s="12"/>
@@ -3569,7 +3550,7 @@
       <c r="K61" s="12"/>
       <c r="L61" s="12"/>
       <c r="M61" s="12"/>
-      <c r="N61" s="13"/>
+      <c r="N61" s="16"/>
       <c r="O61" s="12"/>
       <c r="P61" s="12"/>
       <c r="Q61" s="12"/>
@@ -3600,7 +3581,7 @@
       <c r="K62" s="12"/>
       <c r="L62" s="12"/>
       <c r="M62" s="12"/>
-      <c r="N62" s="13"/>
+      <c r="N62" s="16"/>
       <c r="O62" s="12"/>
       <c r="P62" s="12"/>
       <c r="Q62" s="12"/>
@@ -3631,7 +3612,7 @@
       <c r="K63" s="12"/>
       <c r="L63" s="12"/>
       <c r="M63" s="12"/>
-      <c r="N63" s="13"/>
+      <c r="N63" s="16"/>
       <c r="O63" s="12"/>
       <c r="P63" s="12"/>
       <c r="Q63" s="12"/>
@@ -3662,7 +3643,7 @@
       <c r="K64" s="12"/>
       <c r="L64" s="12"/>
       <c r="M64" s="12"/>
-      <c r="N64" s="13"/>
+      <c r="N64" s="16"/>
       <c r="O64" s="12"/>
       <c r="P64" s="12"/>
       <c r="Q64" s="12"/>
@@ -3693,7 +3674,7 @@
       <c r="K65" s="12"/>
       <c r="L65" s="12"/>
       <c r="M65" s="12"/>
-      <c r="N65" s="13"/>
+      <c r="N65" s="16"/>
       <c r="O65" s="12"/>
       <c r="P65" s="12"/>
       <c r="Q65" s="12"/>
@@ -3724,7 +3705,7 @@
       <c r="K66" s="12"/>
       <c r="L66" s="12"/>
       <c r="M66" s="12"/>
-      <c r="N66" s="13"/>
+      <c r="N66" s="16"/>
       <c r="O66" s="12"/>
       <c r="P66" s="12"/>
       <c r="Q66" s="12"/>
@@ -3755,7 +3736,7 @@
       <c r="K67" s="12"/>
       <c r="L67" s="12"/>
       <c r="M67" s="12"/>
-      <c r="N67" s="13"/>
+      <c r="N67" s="16"/>
       <c r="O67" s="12"/>
       <c r="P67" s="12"/>
       <c r="Q67" s="12"/>
@@ -3786,7 +3767,7 @@
       <c r="K68" s="12"/>
       <c r="L68" s="12"/>
       <c r="M68" s="12"/>
-      <c r="N68" s="13"/>
+      <c r="N68" s="16"/>
       <c r="O68" s="12"/>
       <c r="P68" s="12"/>
       <c r="Q68" s="12"/>
@@ -3817,7 +3798,7 @@
       <c r="K69" s="12"/>
       <c r="L69" s="12"/>
       <c r="M69" s="12"/>
-      <c r="N69" s="13"/>
+      <c r="N69" s="16"/>
       <c r="O69" s="12"/>
       <c r="P69" s="12"/>
       <c r="Q69" s="12"/>
@@ -3848,7 +3829,7 @@
       <c r="K70" s="12"/>
       <c r="L70" s="12"/>
       <c r="M70" s="12"/>
-      <c r="N70" s="13"/>
+      <c r="N70" s="16"/>
       <c r="O70" s="12"/>
       <c r="P70" s="12"/>
       <c r="Q70" s="12"/>
@@ -3879,7 +3860,7 @@
       <c r="K71" s="12"/>
       <c r="L71" s="12"/>
       <c r="M71" s="12"/>
-      <c r="N71" s="13"/>
+      <c r="N71" s="16"/>
       <c r="O71" s="12"/>
       <c r="P71" s="12"/>
       <c r="Q71" s="12"/>
@@ -3910,7 +3891,7 @@
       <c r="K72" s="12"/>
       <c r="L72" s="12"/>
       <c r="M72" s="12"/>
-      <c r="N72" s="13"/>
+      <c r="N72" s="16"/>
       <c r="O72" s="12"/>
       <c r="P72" s="12"/>
       <c r="Q72" s="12"/>
@@ -3941,7 +3922,7 @@
       <c r="K73" s="12"/>
       <c r="L73" s="12"/>
       <c r="M73" s="12"/>
-      <c r="N73" s="13"/>
+      <c r="N73" s="16"/>
       <c r="O73" s="12"/>
       <c r="P73" s="12"/>
       <c r="Q73" s="12"/>
@@ -3972,7 +3953,7 @@
       <c r="K74" s="12"/>
       <c r="L74" s="12"/>
       <c r="M74" s="12"/>
-      <c r="N74" s="13"/>
+      <c r="N74" s="16"/>
       <c r="O74" s="12"/>
       <c r="P74" s="12"/>
       <c r="Q74" s="12"/>
@@ -4003,7 +3984,7 @@
       <c r="K75" s="12"/>
       <c r="L75" s="12"/>
       <c r="M75" s="12"/>
-      <c r="N75" s="13"/>
+      <c r="N75" s="16"/>
       <c r="O75" s="12"/>
       <c r="P75" s="12"/>
       <c r="Q75" s="12"/>
@@ -4034,7 +4015,7 @@
       <c r="K76" s="12"/>
       <c r="L76" s="12"/>
       <c r="M76" s="12"/>
-      <c r="N76" s="13"/>
+      <c r="N76" s="16"/>
       <c r="O76" s="12"/>
       <c r="P76" s="12"/>
       <c r="Q76" s="12"/>
@@ -4065,7 +4046,7 @@
       <c r="K77" s="12"/>
       <c r="L77" s="12"/>
       <c r="M77" s="12"/>
-      <c r="N77" s="13"/>
+      <c r="N77" s="16"/>
       <c r="O77" s="12"/>
       <c r="P77" s="12"/>
       <c r="Q77" s="12"/>
@@ -4096,7 +4077,7 @@
       <c r="K78" s="12"/>
       <c r="L78" s="12"/>
       <c r="M78" s="12"/>
-      <c r="N78" s="13"/>
+      <c r="N78" s="16"/>
       <c r="O78" s="12"/>
       <c r="P78" s="12"/>
       <c r="Q78" s="12"/>
@@ -4127,7 +4108,7 @@
       <c r="K79" s="12"/>
       <c r="L79" s="12"/>
       <c r="M79" s="12"/>
-      <c r="N79" s="13"/>
+      <c r="N79" s="16"/>
       <c r="O79" s="12"/>
       <c r="P79" s="12"/>
       <c r="Q79" s="12"/>
@@ -4158,7 +4139,7 @@
       <c r="K80" s="12"/>
       <c r="L80" s="12"/>
       <c r="M80" s="12"/>
-      <c r="N80" s="13"/>
+      <c r="N80" s="16"/>
       <c r="O80" s="12"/>
       <c r="P80" s="12"/>
       <c r="Q80" s="12"/>
@@ -4189,7 +4170,7 @@
       <c r="K81" s="12"/>
       <c r="L81" s="12"/>
       <c r="M81" s="12"/>
-      <c r="N81" s="13"/>
+      <c r="N81" s="16"/>
       <c r="O81" s="12"/>
       <c r="P81" s="12"/>
       <c r="Q81" s="12"/>
@@ -4220,7 +4201,7 @@
       <c r="K82" s="12"/>
       <c r="L82" s="12"/>
       <c r="M82" s="12"/>
-      <c r="N82" s="13"/>
+      <c r="N82" s="16"/>
       <c r="O82" s="12"/>
       <c r="P82" s="12"/>
       <c r="Q82" s="12"/>
@@ -4251,7 +4232,7 @@
       <c r="K83" s="12"/>
       <c r="L83" s="12"/>
       <c r="M83" s="12"/>
-      <c r="N83" s="13"/>
+      <c r="N83" s="16"/>
       <c r="O83" s="12"/>
       <c r="P83" s="12"/>
       <c r="Q83" s="12"/>
@@ -4282,7 +4263,7 @@
       <c r="K84" s="12"/>
       <c r="L84" s="12"/>
       <c r="M84" s="12"/>
-      <c r="N84" s="13"/>
+      <c r="N84" s="16"/>
       <c r="O84" s="12"/>
       <c r="P84" s="12"/>
       <c r="Q84" s="12"/>
@@ -4313,7 +4294,7 @@
       <c r="K85" s="12"/>
       <c r="L85" s="12"/>
       <c r="M85" s="12"/>
-      <c r="N85" s="13"/>
+      <c r="N85" s="16"/>
       <c r="O85" s="12"/>
       <c r="P85" s="12"/>
       <c r="Q85" s="12"/>
@@ -4344,7 +4325,7 @@
       <c r="K86" s="12"/>
       <c r="L86" s="12"/>
       <c r="M86" s="12"/>
-      <c r="N86" s="13"/>
+      <c r="N86" s="16"/>
       <c r="O86" s="12"/>
       <c r="P86" s="12"/>
       <c r="Q86" s="12"/>
@@ -4375,7 +4356,7 @@
       <c r="K87" s="12"/>
       <c r="L87" s="12"/>
       <c r="M87" s="12"/>
-      <c r="N87" s="13"/>
+      <c r="N87" s="16"/>
       <c r="O87" s="12"/>
       <c r="P87" s="12"/>
       <c r="Q87" s="12"/>
@@ -4406,7 +4387,7 @@
       <c r="K88" s="12"/>
       <c r="L88" s="12"/>
       <c r="M88" s="12"/>
-      <c r="N88" s="13"/>
+      <c r="N88" s="16"/>
       <c r="O88" s="12"/>
       <c r="P88" s="12"/>
       <c r="Q88" s="12"/>
@@ -4437,7 +4418,7 @@
       <c r="K89" s="12"/>
       <c r="L89" s="12"/>
       <c r="M89" s="12"/>
-      <c r="N89" s="13"/>
+      <c r="N89" s="16"/>
       <c r="O89" s="12"/>
       <c r="P89" s="12"/>
       <c r="Q89" s="12"/>
@@ -4468,7 +4449,7 @@
       <c r="K90" s="12"/>
       <c r="L90" s="12"/>
       <c r="M90" s="12"/>
-      <c r="N90" s="13"/>
+      <c r="N90" s="16"/>
       <c r="O90" s="12"/>
       <c r="P90" s="12"/>
       <c r="Q90" s="12"/>
@@ -4499,7 +4480,7 @@
       <c r="K91" s="12"/>
       <c r="L91" s="12"/>
       <c r="M91" s="12"/>
-      <c r="N91" s="13"/>
+      <c r="N91" s="16"/>
       <c r="O91" s="12"/>
       <c r="P91" s="12"/>
       <c r="Q91" s="12"/>
@@ -4530,7 +4511,7 @@
       <c r="K92" s="12"/>
       <c r="L92" s="12"/>
       <c r="M92" s="12"/>
-      <c r="N92" s="13"/>
+      <c r="N92" s="16"/>
       <c r="O92" s="12"/>
       <c r="P92" s="12"/>
       <c r="Q92" s="12"/>
@@ -4561,7 +4542,7 @@
       <c r="K93" s="12"/>
       <c r="L93" s="12"/>
       <c r="M93" s="12"/>
-      <c r="N93" s="13"/>
+      <c r="N93" s="16"/>
       <c r="O93" s="12"/>
       <c r="P93" s="12"/>
       <c r="Q93" s="12"/>
@@ -4592,7 +4573,7 @@
       <c r="K94" s="12"/>
       <c r="L94" s="12"/>
       <c r="M94" s="12"/>
-      <c r="N94" s="13"/>
+      <c r="N94" s="16"/>
       <c r="O94" s="12"/>
       <c r="P94" s="12"/>
       <c r="Q94" s="12"/>
@@ -4623,7 +4604,7 @@
       <c r="K95" s="12"/>
       <c r="L95" s="12"/>
       <c r="M95" s="12"/>
-      <c r="N95" s="13"/>
+      <c r="N95" s="16"/>
       <c r="O95" s="12"/>
       <c r="P95" s="12"/>
       <c r="Q95" s="12"/>
@@ -4654,7 +4635,7 @@
       <c r="K96" s="12"/>
       <c r="L96" s="12"/>
       <c r="M96" s="12"/>
-      <c r="N96" s="13"/>
+      <c r="N96" s="16"/>
       <c r="O96" s="12"/>
       <c r="P96" s="12"/>
       <c r="Q96" s="12"/>
@@ -4685,7 +4666,7 @@
       <c r="K97" s="12"/>
       <c r="L97" s="12"/>
       <c r="M97" s="12"/>
-      <c r="N97" s="13"/>
+      <c r="N97" s="16"/>
       <c r="O97" s="12"/>
       <c r="P97" s="12"/>
       <c r="Q97" s="12"/>
@@ -4716,7 +4697,7 @@
       <c r="K98" s="12"/>
       <c r="L98" s="12"/>
       <c r="M98" s="12"/>
-      <c r="N98" s="13"/>
+      <c r="N98" s="16"/>
       <c r="O98" s="12"/>
       <c r="P98" s="12"/>
       <c r="Q98" s="12"/>
@@ -4747,7 +4728,7 @@
       <c r="K99" s="12"/>
       <c r="L99" s="12"/>
       <c r="M99" s="12"/>
-      <c r="N99" s="13"/>
+      <c r="N99" s="16"/>
       <c r="O99" s="12"/>
       <c r="P99" s="12"/>
       <c r="Q99" s="12"/>
@@ -4778,7 +4759,7 @@
       <c r="K100" s="12"/>
       <c r="L100" s="12"/>
       <c r="M100" s="12"/>
-      <c r="N100" s="13"/>
+      <c r="N100" s="16"/>
       <c r="O100" s="12"/>
       <c r="P100" s="12"/>
       <c r="Q100" s="12"/>
@@ -4809,7 +4790,7 @@
       <c r="K101" s="12"/>
       <c r="L101" s="12"/>
       <c r="M101" s="12"/>
-      <c r="N101" s="13"/>
+      <c r="N101" s="16"/>
       <c r="O101" s="12"/>
       <c r="P101" s="12"/>
       <c r="Q101" s="12"/>
@@ -4840,7 +4821,7 @@
       <c r="K102" s="12"/>
       <c r="L102" s="12"/>
       <c r="M102" s="12"/>
-      <c r="N102" s="13"/>
+      <c r="N102" s="16"/>
       <c r="O102" s="12"/>
       <c r="P102" s="12"/>
       <c r="Q102" s="12"/>
@@ -4871,7 +4852,7 @@
       <c r="K103" s="12"/>
       <c r="L103" s="12"/>
       <c r="M103" s="12"/>
-      <c r="N103" s="13"/>
+      <c r="N103" s="16"/>
       <c r="O103" s="12"/>
       <c r="P103" s="12"/>
       <c r="Q103" s="12"/>
@@ -4902,7 +4883,7 @@
       <c r="K104" s="12"/>
       <c r="L104" s="12"/>
       <c r="M104" s="12"/>
-      <c r="N104" s="13"/>
+      <c r="N104" s="16"/>
       <c r="O104" s="12"/>
       <c r="P104" s="12"/>
       <c r="Q104" s="12"/>
@@ -4933,7 +4914,7 @@
       <c r="K105" s="12"/>
       <c r="L105" s="12"/>
       <c r="M105" s="12"/>
-      <c r="N105" s="13"/>
+      <c r="N105" s="16"/>
       <c r="O105" s="12"/>
       <c r="P105" s="12"/>
       <c r="Q105" s="12"/>
@@ -4964,7 +4945,7 @@
       <c r="K106" s="12"/>
       <c r="L106" s="12"/>
       <c r="M106" s="12"/>
-      <c r="N106" s="13"/>
+      <c r="N106" s="16"/>
       <c r="O106" s="12"/>
       <c r="P106" s="12"/>
       <c r="Q106" s="12"/>
@@ -4995,7 +4976,7 @@
       <c r="K107" s="12"/>
       <c r="L107" s="12"/>
       <c r="M107" s="12"/>
-      <c r="N107" s="13"/>
+      <c r="N107" s="16"/>
       <c r="O107" s="12"/>
       <c r="P107" s="12"/>
       <c r="Q107" s="12"/>
@@ -5026,7 +5007,7 @@
       <c r="K108" s="12"/>
       <c r="L108" s="12"/>
       <c r="M108" s="12"/>
-      <c r="N108" s="13"/>
+      <c r="N108" s="16"/>
       <c r="O108" s="12"/>
       <c r="P108" s="12"/>
       <c r="Q108" s="12"/>
@@ -5057,7 +5038,7 @@
       <c r="K109" s="12"/>
       <c r="L109" s="12"/>
       <c r="M109" s="12"/>
-      <c r="N109" s="13"/>
+      <c r="N109" s="16"/>
       <c r="O109" s="12"/>
       <c r="P109" s="12"/>
       <c r="Q109" s="12"/>
@@ -5088,7 +5069,7 @@
       <c r="K110" s="12"/>
       <c r="L110" s="12"/>
       <c r="M110" s="12"/>
-      <c r="N110" s="13"/>
+      <c r="N110" s="16"/>
       <c r="O110" s="12"/>
       <c r="P110" s="12"/>
       <c r="Q110" s="12"/>
@@ -5119,7 +5100,7 @@
       <c r="K111" s="12"/>
       <c r="L111" s="12"/>
       <c r="M111" s="12"/>
-      <c r="N111" s="13"/>
+      <c r="N111" s="16"/>
       <c r="O111" s="12"/>
       <c r="P111" s="12"/>
       <c r="Q111" s="12"/>
@@ -5150,7 +5131,7 @@
       <c r="K112" s="12"/>
       <c r="L112" s="12"/>
       <c r="M112" s="12"/>
-      <c r="N112" s="13"/>
+      <c r="N112" s="16"/>
       <c r="O112" s="12"/>
       <c r="P112" s="12"/>
       <c r="Q112" s="12"/>
@@ -5181,7 +5162,7 @@
       <c r="K113" s="12"/>
       <c r="L113" s="12"/>
       <c r="M113" s="12"/>
-      <c r="N113" s="13"/>
+      <c r="N113" s="16"/>
       <c r="O113" s="12"/>
       <c r="P113" s="12"/>
       <c r="Q113" s="12"/>
@@ -5212,7 +5193,7 @@
       <c r="K114" s="12"/>
       <c r="L114" s="12"/>
       <c r="M114" s="12"/>
-      <c r="N114" s="13"/>
+      <c r="N114" s="16"/>
       <c r="O114" s="12"/>
       <c r="P114" s="12"/>
       <c r="Q114" s="12"/>
@@ -5243,7 +5224,7 @@
       <c r="K115" s="12"/>
       <c r="L115" s="12"/>
       <c r="M115" s="12"/>
-      <c r="N115" s="13"/>
+      <c r="N115" s="16"/>
       <c r="O115" s="12"/>
       <c r="P115" s="12"/>
       <c r="Q115" s="12"/>
@@ -5274,7 +5255,7 @@
       <c r="K116" s="12"/>
       <c r="L116" s="12"/>
       <c r="M116" s="12"/>
-      <c r="N116" s="13"/>
+      <c r="N116" s="16"/>
       <c r="O116" s="12"/>
       <c r="P116" s="12"/>
       <c r="Q116" s="12"/>
@@ -5305,7 +5286,7 @@
       <c r="K117" s="12"/>
       <c r="L117" s="12"/>
       <c r="M117" s="12"/>
-      <c r="N117" s="13"/>
+      <c r="N117" s="16"/>
       <c r="O117" s="12"/>
       <c r="P117" s="12"/>
       <c r="Q117" s="12"/>
@@ -5336,7 +5317,7 @@
       <c r="K118" s="12"/>
       <c r="L118" s="12"/>
       <c r="M118" s="12"/>
-      <c r="N118" s="13"/>
+      <c r="N118" s="16"/>
       <c r="O118" s="12"/>
       <c r="P118" s="12"/>
       <c r="Q118" s="12"/>
@@ -5367,7 +5348,7 @@
       <c r="K119" s="12"/>
       <c r="L119" s="12"/>
       <c r="M119" s="12"/>
-      <c r="N119" s="13"/>
+      <c r="N119" s="16"/>
       <c r="O119" s="12"/>
       <c r="P119" s="12"/>
       <c r="Q119" s="12"/>
@@ -5398,7 +5379,7 @@
       <c r="K120" s="12"/>
       <c r="L120" s="12"/>
       <c r="M120" s="12"/>
-      <c r="N120" s="13"/>
+      <c r="N120" s="16"/>
       <c r="O120" s="12"/>
       <c r="P120" s="12"/>
       <c r="Q120" s="12"/>
@@ -5429,7 +5410,7 @@
       <c r="K121" s="12"/>
       <c r="L121" s="12"/>
       <c r="M121" s="12"/>
-      <c r="N121" s="13"/>
+      <c r="N121" s="16"/>
       <c r="O121" s="12"/>
       <c r="P121" s="12"/>
       <c r="Q121" s="12"/>
@@ -5460,7 +5441,7 @@
       <c r="K122" s="12"/>
       <c r="L122" s="12"/>
       <c r="M122" s="12"/>
-      <c r="N122" s="13"/>
+      <c r="N122" s="16"/>
       <c r="O122" s="12"/>
       <c r="P122" s="12"/>
       <c r="Q122" s="12"/>
@@ -5491,7 +5472,7 @@
       <c r="K123" s="12"/>
       <c r="L123" s="12"/>
       <c r="M123" s="12"/>
-      <c r="N123" s="13"/>
+      <c r="N123" s="16"/>
       <c r="O123" s="12"/>
       <c r="P123" s="12"/>
       <c r="Q123" s="12"/>
@@ -5522,7 +5503,7 @@
       <c r="K124" s="12"/>
       <c r="L124" s="12"/>
       <c r="M124" s="12"/>
-      <c r="N124" s="13"/>
+      <c r="N124" s="16"/>
       <c r="O124" s="12"/>
       <c r="P124" s="12"/>
       <c r="Q124" s="12"/>
@@ -5553,7 +5534,7 @@
       <c r="K125" s="12"/>
       <c r="L125" s="12"/>
       <c r="M125" s="12"/>
-      <c r="N125" s="13"/>
+      <c r="N125" s="16"/>
       <c r="O125" s="12"/>
       <c r="P125" s="12"/>
       <c r="Q125" s="12"/>
@@ -5584,7 +5565,7 @@
       <c r="K126" s="12"/>
       <c r="L126" s="12"/>
       <c r="M126" s="12"/>
-      <c r="N126" s="13"/>
+      <c r="N126" s="16"/>
       <c r="O126" s="12"/>
       <c r="P126" s="12"/>
       <c r="Q126" s="12"/>
@@ -5615,7 +5596,7 @@
       <c r="K127" s="12"/>
       <c r="L127" s="12"/>
       <c r="M127" s="12"/>
-      <c r="N127" s="13"/>
+      <c r="N127" s="16"/>
       <c r="O127" s="12"/>
       <c r="P127" s="12"/>
       <c r="Q127" s="12"/>
@@ -5646,7 +5627,7 @@
       <c r="K128" s="12"/>
       <c r="L128" s="12"/>
       <c r="M128" s="12"/>
-      <c r="N128" s="13"/>
+      <c r="N128" s="16"/>
       <c r="O128" s="12"/>
       <c r="P128" s="12"/>
       <c r="Q128" s="12"/>
@@ -5677,7 +5658,7 @@
       <c r="K129" s="12"/>
       <c r="L129" s="12"/>
       <c r="M129" s="12"/>
-      <c r="N129" s="13"/>
+      <c r="N129" s="16"/>
       <c r="O129" s="12"/>
       <c r="P129" s="12"/>
       <c r="Q129" s="12"/>
@@ -5708,7 +5689,7 @@
       <c r="K130" s="12"/>
       <c r="L130" s="12"/>
       <c r="M130" s="12"/>
-      <c r="N130" s="13"/>
+      <c r="N130" s="16"/>
       <c r="O130" s="12"/>
       <c r="P130" s="12"/>
       <c r="Q130" s="12"/>
@@ -5739,7 +5720,7 @@
       <c r="K131" s="12"/>
       <c r="L131" s="12"/>
       <c r="M131" s="12"/>
-      <c r="N131" s="13"/>
+      <c r="N131" s="16"/>
       <c r="O131" s="12"/>
       <c r="P131" s="12"/>
       <c r="Q131" s="12"/>
@@ -5770,7 +5751,7 @@
       <c r="K132" s="12"/>
       <c r="L132" s="12"/>
       <c r="M132" s="12"/>
-      <c r="N132" s="13"/>
+      <c r="N132" s="16"/>
       <c r="O132" s="12"/>
       <c r="P132" s="12"/>
       <c r="Q132" s="12"/>
@@ -5801,7 +5782,7 @@
       <c r="K133" s="12"/>
       <c r="L133" s="12"/>
       <c r="M133" s="12"/>
-      <c r="N133" s="13"/>
+      <c r="N133" s="16"/>
       <c r="O133" s="12"/>
       <c r="P133" s="12"/>
       <c r="Q133" s="12"/>
@@ -5832,7 +5813,7 @@
       <c r="K134" s="12"/>
       <c r="L134" s="12"/>
       <c r="M134" s="12"/>
-      <c r="N134" s="13"/>
+      <c r="N134" s="16"/>
       <c r="O134" s="12"/>
       <c r="P134" s="12"/>
       <c r="Q134" s="12"/>
@@ -5863,7 +5844,7 @@
       <c r="K135" s="12"/>
       <c r="L135" s="12"/>
       <c r="M135" s="12"/>
-      <c r="N135" s="13"/>
+      <c r="N135" s="16"/>
       <c r="O135" s="12"/>
       <c r="P135" s="12"/>
       <c r="Q135" s="12"/>
@@ -5894,7 +5875,7 @@
       <c r="K136" s="12"/>
       <c r="L136" s="12"/>
       <c r="M136" s="12"/>
-      <c r="N136" s="13"/>
+      <c r="N136" s="16"/>
       <c r="O136" s="12"/>
       <c r="P136" s="12"/>
       <c r="Q136" s="12"/>
@@ -5925,7 +5906,7 @@
       <c r="K137" s="12"/>
       <c r="L137" s="12"/>
       <c r="M137" s="12"/>
-      <c r="N137" s="13"/>
+      <c r="N137" s="16"/>
       <c r="O137" s="12"/>
       <c r="P137" s="12"/>
       <c r="Q137" s="12"/>
@@ -5956,7 +5937,7 @@
       <c r="K138" s="12"/>
       <c r="L138" s="12"/>
       <c r="M138" s="12"/>
-      <c r="N138" s="13"/>
+      <c r="N138" s="16"/>
       <c r="O138" s="12"/>
       <c r="P138" s="12"/>
       <c r="Q138" s="12"/>
@@ -5987,7 +5968,7 @@
       <c r="K139" s="12"/>
       <c r="L139" s="12"/>
       <c r="M139" s="12"/>
-      <c r="N139" s="13"/>
+      <c r="N139" s="16"/>
       <c r="O139" s="12"/>
       <c r="P139" s="12"/>
       <c r="Q139" s="12"/>
@@ -6018,7 +5999,7 @@
       <c r="K140" s="12"/>
       <c r="L140" s="12"/>
       <c r="M140" s="12"/>
-      <c r="N140" s="13"/>
+      <c r="N140" s="16"/>
       <c r="O140" s="12"/>
       <c r="P140" s="12"/>
       <c r="Q140" s="12"/>
@@ -6049,7 +6030,7 @@
       <c r="K141" s="12"/>
       <c r="L141" s="12"/>
       <c r="M141" s="12"/>
-      <c r="N141" s="13"/>
+      <c r="N141" s="16"/>
       <c r="O141" s="12"/>
       <c r="P141" s="12"/>
       <c r="Q141" s="12"/>
@@ -6080,7 +6061,7 @@
       <c r="K142" s="12"/>
       <c r="L142" s="12"/>
       <c r="M142" s="12"/>
-      <c r="N142" s="13"/>
+      <c r="N142" s="16"/>
       <c r="O142" s="12"/>
       <c r="P142" s="12"/>
       <c r="Q142" s="12"/>
@@ -6111,7 +6092,7 @@
       <c r="K143" s="12"/>
       <c r="L143" s="12"/>
       <c r="M143" s="12"/>
-      <c r="N143" s="13"/>
+      <c r="N143" s="16"/>
       <c r="O143" s="12"/>
       <c r="P143" s="12"/>
       <c r="Q143" s="12"/>
@@ -6142,7 +6123,7 @@
       <c r="K144" s="12"/>
       <c r="L144" s="12"/>
       <c r="M144" s="12"/>
-      <c r="N144" s="13"/>
+      <c r="N144" s="16"/>
       <c r="O144" s="12"/>
       <c r="P144" s="12"/>
       <c r="Q144" s="12"/>
@@ -6173,7 +6154,7 @@
       <c r="K145" s="12"/>
       <c r="L145" s="12"/>
       <c r="M145" s="12"/>
-      <c r="N145" s="13"/>
+      <c r="N145" s="16"/>
       <c r="O145" s="12"/>
       <c r="P145" s="12"/>
       <c r="Q145" s="12"/>
@@ -6204,7 +6185,7 @@
       <c r="K146" s="12"/>
       <c r="L146" s="12"/>
       <c r="M146" s="12"/>
-      <c r="N146" s="13"/>
+      <c r="N146" s="16"/>
       <c r="O146" s="12"/>
       <c r="P146" s="12"/>
       <c r="Q146" s="12"/>
@@ -6235,7 +6216,7 @@
       <c r="K147" s="12"/>
       <c r="L147" s="12"/>
       <c r="M147" s="12"/>
-      <c r="N147" s="13"/>
+      <c r="N147" s="16"/>
       <c r="O147" s="12"/>
       <c r="P147" s="12"/>
       <c r="Q147" s="12"/>
@@ -6266,7 +6247,7 @@
       <c r="K148" s="12"/>
       <c r="L148" s="12"/>
       <c r="M148" s="12"/>
-      <c r="N148" s="13"/>
+      <c r="N148" s="16"/>
       <c r="O148" s="12"/>
       <c r="P148" s="12"/>
       <c r="Q148" s="12"/>
@@ -6297,7 +6278,7 @@
       <c r="K149" s="12"/>
       <c r="L149" s="12"/>
       <c r="M149" s="12"/>
-      <c r="N149" s="13"/>
+      <c r="N149" s="16"/>
       <c r="O149" s="12"/>
       <c r="P149" s="12"/>
       <c r="Q149" s="12"/>
@@ -6328,7 +6309,7 @@
       <c r="K150" s="12"/>
       <c r="L150" s="12"/>
       <c r="M150" s="12"/>
-      <c r="N150" s="13"/>
+      <c r="N150" s="16"/>
       <c r="O150" s="12"/>
       <c r="P150" s="12"/>
       <c r="Q150" s="12"/>
@@ -6359,7 +6340,7 @@
       <c r="K151" s="12"/>
       <c r="L151" s="12"/>
       <c r="M151" s="12"/>
-      <c r="N151" s="13"/>
+      <c r="N151" s="16"/>
       <c r="O151" s="12"/>
       <c r="P151" s="12"/>
       <c r="Q151" s="12"/>
@@ -6390,7 +6371,7 @@
       <c r="K152" s="12"/>
       <c r="L152" s="12"/>
       <c r="M152" s="12"/>
-      <c r="N152" s="13"/>
+      <c r="N152" s="16"/>
       <c r="O152" s="12"/>
       <c r="P152" s="12"/>
       <c r="Q152" s="12"/>
@@ -6421,7 +6402,7 @@
       <c r="K153" s="12"/>
       <c r="L153" s="12"/>
       <c r="M153" s="12"/>
-      <c r="N153" s="13"/>
+      <c r="N153" s="16"/>
       <c r="O153" s="12"/>
       <c r="P153" s="12"/>
       <c r="Q153" s="12"/>
@@ -6452,7 +6433,7 @@
       <c r="K154" s="12"/>
       <c r="L154" s="12"/>
       <c r="M154" s="12"/>
-      <c r="N154" s="13"/>
+      <c r="N154" s="16"/>
       <c r="O154" s="12"/>
       <c r="P154" s="12"/>
       <c r="Q154" s="12"/>
@@ -6483,7 +6464,7 @@
       <c r="K155" s="12"/>
       <c r="L155" s="12"/>
       <c r="M155" s="12"/>
-      <c r="N155" s="13"/>
+      <c r="N155" s="16"/>
       <c r="O155" s="12"/>
       <c r="P155" s="12"/>
       <c r="Q155" s="12"/>
@@ -6514,7 +6495,7 @@
       <c r="K156" s="12"/>
       <c r="L156" s="12"/>
       <c r="M156" s="12"/>
-      <c r="N156" s="13"/>
+      <c r="N156" s="16"/>
       <c r="O156" s="12"/>
       <c r="P156" s="12"/>
       <c r="Q156" s="12"/>
@@ -6545,7 +6526,7 @@
       <c r="K157" s="12"/>
       <c r="L157" s="12"/>
       <c r="M157" s="12"/>
-      <c r="N157" s="13"/>
+      <c r="N157" s="16"/>
       <c r="O157" s="12"/>
       <c r="P157" s="12"/>
       <c r="Q157" s="12"/>
@@ -6576,7 +6557,7 @@
       <c r="K158" s="12"/>
       <c r="L158" s="12"/>
       <c r="M158" s="12"/>
-      <c r="N158" s="13"/>
+      <c r="N158" s="16"/>
       <c r="O158" s="12"/>
       <c r="P158" s="12"/>
       <c r="Q158" s="12"/>
@@ -6607,7 +6588,7 @@
       <c r="K159" s="12"/>
       <c r="L159" s="12"/>
       <c r="M159" s="12"/>
-      <c r="N159" s="13"/>
+      <c r="N159" s="16"/>
       <c r="O159" s="12"/>
       <c r="P159" s="12"/>
       <c r="Q159" s="12"/>
@@ -6638,7 +6619,7 @@
       <c r="K160" s="12"/>
       <c r="L160" s="12"/>
       <c r="M160" s="12"/>
-      <c r="N160" s="13"/>
+      <c r="N160" s="16"/>
       <c r="O160" s="12"/>
       <c r="P160" s="12"/>
       <c r="Q160" s="12"/>
@@ -6669,7 +6650,7 @@
       <c r="K161" s="12"/>
       <c r="L161" s="12"/>
       <c r="M161" s="12"/>
-      <c r="N161" s="13"/>
+      <c r="N161" s="16"/>
       <c r="O161" s="12"/>
       <c r="P161" s="12"/>
       <c r="Q161" s="12"/>
@@ -6700,7 +6681,7 @@
       <c r="K162" s="12"/>
       <c r="L162" s="12"/>
       <c r="M162" s="12"/>
-      <c r="N162" s="13"/>
+      <c r="N162" s="16"/>
       <c r="O162" s="12"/>
       <c r="P162" s="12"/>
       <c r="Q162" s="12"/>
@@ -6731,7 +6712,7 @@
       <c r="K163" s="12"/>
       <c r="L163" s="12"/>
       <c r="M163" s="12"/>
-      <c r="N163" s="13"/>
+      <c r="N163" s="16"/>
       <c r="O163" s="12"/>
       <c r="P163" s="12"/>
       <c r="Q163" s="12"/>
@@ -6762,7 +6743,7 @@
       <c r="K164" s="12"/>
       <c r="L164" s="12"/>
       <c r="M164" s="12"/>
-      <c r="N164" s="13"/>
+      <c r="N164" s="16"/>
       <c r="O164" s="12"/>
       <c r="P164" s="12"/>
       <c r="Q164" s="12"/>
@@ -6793,7 +6774,7 @@
       <c r="K165" s="12"/>
       <c r="L165" s="12"/>
       <c r="M165" s="12"/>
-      <c r="N165" s="13"/>
+      <c r="N165" s="16"/>
       <c r="O165" s="12"/>
       <c r="P165" s="12"/>
       <c r="Q165" s="12"/>
@@ -6824,7 +6805,7 @@
       <c r="K166" s="12"/>
       <c r="L166" s="12"/>
       <c r="M166" s="12"/>
-      <c r="N166" s="13"/>
+      <c r="N166" s="16"/>
       <c r="O166" s="12"/>
       <c r="P166" s="12"/>
       <c r="Q166" s="12"/>
@@ -6855,7 +6836,7 @@
       <c r="K167" s="12"/>
       <c r="L167" s="12"/>
       <c r="M167" s="12"/>
-      <c r="N167" s="13"/>
+      <c r="N167" s="16"/>
       <c r="O167" s="12"/>
       <c r="P167" s="12"/>
       <c r="Q167" s="12"/>
@@ -6886,7 +6867,7 @@
       <c r="K168" s="12"/>
       <c r="L168" s="12"/>
       <c r="M168" s="12"/>
-      <c r="N168" s="13"/>
+      <c r="N168" s="16"/>
       <c r="O168" s="12"/>
       <c r="P168" s="12"/>
       <c r="Q168" s="12"/>
@@ -6917,7 +6898,7 @@
       <c r="K169" s="12"/>
       <c r="L169" s="12"/>
       <c r="M169" s="12"/>
-      <c r="N169" s="13"/>
+      <c r="N169" s="16"/>
       <c r="O169" s="12"/>
       <c r="P169" s="12"/>
       <c r="Q169" s="12"/>
@@ -6948,7 +6929,7 @@
       <c r="K170" s="12"/>
       <c r="L170" s="12"/>
       <c r="M170" s="12"/>
-      <c r="N170" s="13"/>
+      <c r="N170" s="16"/>
       <c r="O170" s="12"/>
       <c r="P170" s="12"/>
       <c r="Q170" s="12"/>
@@ -6979,7 +6960,7 @@
       <c r="K171" s="12"/>
       <c r="L171" s="12"/>
       <c r="M171" s="12"/>
-      <c r="N171" s="13"/>
+      <c r="N171" s="16"/>
       <c r="O171" s="12"/>
       <c r="P171" s="12"/>
       <c r="Q171" s="12"/>
@@ -7010,7 +6991,7 @@
       <c r="K172" s="12"/>
       <c r="L172" s="12"/>
       <c r="M172" s="12"/>
-      <c r="N172" s="13"/>
+      <c r="N172" s="16"/>
       <c r="O172" s="12"/>
       <c r="P172" s="12"/>
       <c r="Q172" s="12"/>
@@ -7041,7 +7022,7 @@
       <c r="K173" s="12"/>
       <c r="L173" s="12"/>
       <c r="M173" s="12"/>
-      <c r="N173" s="13"/>
+      <c r="N173" s="16"/>
       <c r="O173" s="12"/>
       <c r="P173" s="12"/>
       <c r="Q173" s="12"/>
@@ -7072,7 +7053,7 @@
       <c r="K174" s="12"/>
       <c r="L174" s="12"/>
       <c r="M174" s="12"/>
-      <c r="N174" s="13"/>
+      <c r="N174" s="16"/>
       <c r="O174" s="12"/>
       <c r="P174" s="12"/>
       <c r="Q174" s="12"/>
@@ -7103,7 +7084,7 @@
       <c r="K175" s="12"/>
       <c r="L175" s="12"/>
       <c r="M175" s="12"/>
-      <c r="N175" s="13"/>
+      <c r="N175" s="16"/>
       <c r="O175" s="12"/>
       <c r="P175" s="12"/>
       <c r="Q175" s="12"/>
@@ -7134,7 +7115,7 @@
       <c r="K176" s="12"/>
       <c r="L176" s="12"/>
       <c r="M176" s="12"/>
-      <c r="N176" s="13"/>
+      <c r="N176" s="16"/>
       <c r="O176" s="12"/>
       <c r="P176" s="12"/>
       <c r="Q176" s="12"/>
@@ -7165,7 +7146,7 @@
       <c r="K177" s="12"/>
       <c r="L177" s="12"/>
       <c r="M177" s="12"/>
-      <c r="N177" s="13"/>
+      <c r="N177" s="16"/>
       <c r="O177" s="12"/>
       <c r="P177" s="12"/>
       <c r="Q177" s="12"/>
@@ -7196,7 +7177,7 @@
       <c r="K178" s="12"/>
       <c r="L178" s="12"/>
       <c r="M178" s="12"/>
-      <c r="N178" s="13"/>
+      <c r="N178" s="16"/>
       <c r="O178" s="12"/>
       <c r="P178" s="12"/>
       <c r="Q178" s="12"/>
@@ -7227,7 +7208,7 @@
       <c r="K179" s="12"/>
       <c r="L179" s="12"/>
       <c r="M179" s="12"/>
-      <c r="N179" s="13"/>
+      <c r="N179" s="16"/>
       <c r="O179" s="12"/>
       <c r="P179" s="12"/>
       <c r="Q179" s="12"/>
@@ -7258,7 +7239,7 @@
       <c r="K180" s="12"/>
       <c r="L180" s="12"/>
       <c r="M180" s="12"/>
-      <c r="N180" s="13"/>
+      <c r="N180" s="16"/>
       <c r="O180" s="12"/>
       <c r="P180" s="12"/>
       <c r="Q180" s="12"/>
@@ -7289,7 +7270,7 @@
       <c r="K181" s="12"/>
       <c r="L181" s="12"/>
       <c r="M181" s="12"/>
-      <c r="N181" s="13"/>
+      <c r="N181" s="16"/>
       <c r="O181" s="12"/>
       <c r="P181" s="12"/>
       <c r="Q181" s="12"/>
@@ -7320,7 +7301,7 @@
       <c r="K182" s="12"/>
       <c r="L182" s="12"/>
       <c r="M182" s="12"/>
-      <c r="N182" s="13"/>
+      <c r="N182" s="16"/>
       <c r="O182" s="12"/>
       <c r="P182" s="12"/>
       <c r="Q182" s="12"/>
@@ -7351,7 +7332,7 @@
       <c r="K183" s="12"/>
       <c r="L183" s="12"/>
       <c r="M183" s="12"/>
-      <c r="N183" s="13"/>
+      <c r="N183" s="16"/>
       <c r="O183" s="12"/>
       <c r="P183" s="12"/>
       <c r="Q183" s="12"/>
@@ -7382,7 +7363,7 @@
       <c r="K184" s="12"/>
       <c r="L184" s="12"/>
       <c r="M184" s="12"/>
-      <c r="N184" s="13"/>
+      <c r="N184" s="16"/>
       <c r="O184" s="12"/>
       <c r="P184" s="12"/>
       <c r="Q184" s="12"/>
@@ -7413,7 +7394,7 @@
       <c r="K185" s="12"/>
       <c r="L185" s="12"/>
       <c r="M185" s="12"/>
-      <c r="N185" s="13"/>
+      <c r="N185" s="16"/>
       <c r="O185" s="12"/>
       <c r="P185" s="12"/>
       <c r="Q185" s="12"/>
@@ -7444,7 +7425,7 @@
       <c r="K186" s="12"/>
       <c r="L186" s="12"/>
       <c r="M186" s="12"/>
-      <c r="N186" s="13"/>
+      <c r="N186" s="16"/>
       <c r="O186" s="12"/>
       <c r="P186" s="12"/>
       <c r="Q186" s="12"/>
@@ -7475,7 +7456,7 @@
       <c r="K187" s="12"/>
       <c r="L187" s="12"/>
       <c r="M187" s="12"/>
-      <c r="N187" s="13"/>
+      <c r="N187" s="16"/>
       <c r="O187" s="12"/>
       <c r="P187" s="12"/>
       <c r="Q187" s="12"/>
@@ -7506,7 +7487,7 @@
       <c r="K188" s="12"/>
       <c r="L188" s="12"/>
       <c r="M188" s="12"/>
-      <c r="N188" s="13"/>
+      <c r="N188" s="16"/>
       <c r="O188" s="12"/>
       <c r="P188" s="12"/>
       <c r="Q188" s="12"/>
@@ -7537,7 +7518,7 @@
       <c r="K189" s="12"/>
       <c r="L189" s="12"/>
       <c r="M189" s="12"/>
-      <c r="N189" s="13"/>
+      <c r="N189" s="16"/>
       <c r="O189" s="12"/>
       <c r="P189" s="12"/>
       <c r="Q189" s="12"/>
@@ -7568,7 +7549,7 @@
       <c r="K190" s="12"/>
       <c r="L190" s="12"/>
       <c r="M190" s="12"/>
-      <c r="N190" s="13"/>
+      <c r="N190" s="16"/>
       <c r="O190" s="12"/>
       <c r="P190" s="12"/>
       <c r="Q190" s="12"/>
@@ -7599,7 +7580,7 @@
       <c r="K191" s="12"/>
       <c r="L191" s="12"/>
       <c r="M191" s="12"/>
-      <c r="N191" s="13"/>
+      <c r="N191" s="16"/>
       <c r="O191" s="12"/>
       <c r="P191" s="12"/>
       <c r="Q191" s="12"/>
@@ -7630,7 +7611,7 @@
       <c r="K192" s="12"/>
       <c r="L192" s="12"/>
       <c r="M192" s="12"/>
-      <c r="N192" s="13"/>
+      <c r="N192" s="16"/>
       <c r="O192" s="12"/>
       <c r="P192" s="12"/>
       <c r="Q192" s="12"/>
@@ -7661,7 +7642,7 @@
       <c r="K193" s="12"/>
       <c r="L193" s="12"/>
       <c r="M193" s="12"/>
-      <c r="N193" s="13"/>
+      <c r="N193" s="16"/>
       <c r="O193" s="12"/>
       <c r="P193" s="12"/>
       <c r="Q193" s="12"/>
@@ -7692,7 +7673,7 @@
       <c r="K194" s="12"/>
       <c r="L194" s="12"/>
       <c r="M194" s="12"/>
-      <c r="N194" s="13"/>
+      <c r="N194" s="16"/>
       <c r="O194" s="12"/>
       <c r="P194" s="12"/>
       <c r="Q194" s="12"/>
@@ -7723,7 +7704,7 @@
       <c r="K195" s="12"/>
       <c r="L195" s="12"/>
       <c r="M195" s="12"/>
-      <c r="N195" s="13"/>
+      <c r="N195" s="16"/>
       <c r="O195" s="12"/>
       <c r="P195" s="12"/>
       <c r="Q195" s="12"/>
@@ -7754,7 +7735,7 @@
       <c r="K196" s="12"/>
       <c r="L196" s="12"/>
       <c r="M196" s="12"/>
-      <c r="N196" s="13"/>
+      <c r="N196" s="16"/>
       <c r="O196" s="12"/>
       <c r="P196" s="12"/>
       <c r="Q196" s="12"/>
@@ -7773,14 +7754,14 @@
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N3:N196">
-      <formula1>"妈妈,爸爸,奶奶,爷爷,外婆,外公,其他"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:B196">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:B196">
       <formula1>"待产期,已出生"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D4:D196">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5:D196">
       <formula1>"男,女,未知"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N5:N196">
+      <formula1>"妈妈,爸爸,奶奶,爷爷,外婆,外公,其他"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
style: baby management UI
</commit_message>
<xml_diff>
--- a/public/static/template/import_baby_en.xlsx
+++ b/public/static/template/import_baby_en.xlsx
@@ -25,7 +25,7 @@
     <t>Gender</t>
   </si>
   <si>
-    <t>Due Day</t>
+    <t>Due Date</t>
   </si>
   <si>
     <t>Birth Day</t>
@@ -356,7 +356,7 @@
     </r>
   </si>
   <si>
-    <t>Wechat</t>
+    <t>WeChat/WhatApp/Telegram/…</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
fix: update import baby template
</commit_message>
<xml_diff>
--- a/public/static/template/import_baby_en.xlsx
+++ b/public/static/template/import_baby_en.xlsx
@@ -31,7 +31,7 @@
     <t>Birth Day</t>
   </si>
   <si>
-    <t>Infant Supplementary food</t>
+    <t>Infant Supplementary Food</t>
   </si>
   <si>
     <t>Feeding Methods</t>
@@ -170,12 +170,12 @@
   </si>
   <si>
     <t xml:space="preserve">1.Required for EDC
-2.The due date is greater than the current date.
+2.Due date should be after the current date.
 3.Format：YYYY-MM-DD </t>
   </si>
   <si>
     <t>1.Required for born babies.
-2.Birthday is less than the current date.
+2.Birth day should be before the current date.
 3. Format：YYYY-MM-DD</t>
   </si>
   <si>
@@ -356,7 +356,7 @@
     </r>
   </si>
   <si>
-    <t>WeChat/WhatApp/Telegram/…</t>
+    <t>WhatsApp/Telegram/Skype or other instant messaging account</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
[HF-87][Zhenjia Zhou]feat: update excel template
</commit_message>
<xml_diff>
--- a/public/static/template/import_baby_en.xlsx
+++ b/public/static/template/import_baby_en.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ztang/workspace/unc/src/visit-link-admin-web/public/static/template/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhenjia.zhouthoughtworks.com/health-future-admin-frontend/public/static/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A512D797-AA8A-A84D-B6EB-E937DE8930D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93260AEE-3753-CE43-B213-20A0FE89EF23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="30580" windowHeight="19560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -127,46 +127,6 @@
         <rFont val="Monaco"/>
         <family val="2"/>
       </rPr>
-      <t>2.Options:EDC</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="12"/>
-        <rFont val="Monaco"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Monaco"/>
-        <family val="2"/>
-      </rPr>
-      <t>/Birth</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Monaco"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">1.Required
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Monaco"/>
-        <family val="2"/>
-      </rPr>
       <t>2.Options：Male/Female/Unknown</t>
     </r>
     <r>
@@ -191,24 +151,49 @@
 3. Format：YYYY-MM-DD</t>
   </si>
   <si>
+    <t>1.Required</t>
+  </si>
+  <si>
+    <t>1.CHW ID must exist.</t>
+  </si>
+  <si>
+    <t>WhatsApp/Telegram/Skype or other instant messaging account</t>
+  </si>
+  <si>
+    <t>1.Required
+2.Validation:
+Only allow 1-50 characters without special characters</t>
+  </si>
+  <si>
+    <t>1.Required
+2.Validation
+Only allow 1-50 characters without special characters</t>
+  </si>
+  <si>
+    <t>1.Required
+2.Validation
+Only allow 5-20 numbers.</t>
+  </si>
+  <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Monaco"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">1.Optional for born babies.
-</t>
+      <t>1.Optional for born babies.
+2.Options：Exclusive Breastfeeding|| Formula Feeding || Mixed Breast/Formula Feeding || No Breast/Formula Feeding/</t>
     </r>
     <r>
       <rPr>
         <sz val="11"/>
-        <color indexed="8"/>
+        <color indexed="12"/>
         <rFont val="Monaco"/>
         <family val="2"/>
       </rPr>
-      <t>2.Options：Add</t>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>1.Required
+2.Options:Born</t>
     </r>
     <r>
       <rPr>
@@ -227,170 +212,17 @@
         <rFont val="Monaco"/>
         <family val="2"/>
       </rPr>
-      <t>/No Add</t>
+      <t>/Birth</t>
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Monaco"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">1.Optional for born babies.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Monaco"/>
-        <family val="2"/>
-      </rPr>
-      <t>2.Options：Breast Milk/Milk Powder/Mixed/Terminated</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="12"/>
-        <rFont val="Monaco"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
+    <t>1.Optional for born babies.
+2.Options：Add/No Add</t>
   </si>
   <si>
-    <t>1.Required</t>
-  </si>
-  <si>
-    <t>1.CHW ID must exist.</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Monaco"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">1.Required
+    <t xml:space="preserve">1.Required
+2.Relatives Options: Mother/Father/Paternal Grandmother/Maternal Grandmother/Paternal Grandfather/Maternal Grandfather
 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Monaco"/>
-        <family val="2"/>
-      </rPr>
-      <t>2.Relatives Options: Mother/Father/Grandmother</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="12"/>
-        <rFont val="Monaco"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Monaco"/>
-        <family val="2"/>
-      </rPr>
-      <t>/Grandma</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="12"/>
-        <rFont val="Monaco"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Monaco"/>
-        <family val="2"/>
-      </rPr>
-      <t>/Grandfather</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="12"/>
-        <rFont val="Monaco"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Monaco"/>
-        <family val="2"/>
-      </rPr>
-      <t>/Grandpa</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="12"/>
-        <rFont val="Monaco"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Monaco"/>
-        <family val="2"/>
-      </rPr>
-      <t>/Other</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="12"/>
-        <rFont val="Monaco"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-  </si>
-  <si>
-    <t>WhatsApp/Telegram/Skype or other instant messaging account</t>
-  </si>
-  <si>
-    <t>1.Required
-2.Validation:
-Only allow 1-50 characters without special characters</t>
-  </si>
-  <si>
-    <t>1.Required
-2.Validation
-Only allow 1-50 characters without special characters</t>
-  </si>
-  <si>
-    <t>1.Required
-2.Validation
-Only allow 5-20 numbers.</t>
   </si>
 </sst>
 </file>
@@ -1650,8 +1482,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AC196"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="O14" sqref="O14"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13.75" customHeight="1"/>
@@ -1780,47 +1612,47 @@
         <v>28</v>
       </c>
       <c r="B2" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D2" s="6" t="s">
+      <c r="E2" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="F2" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="G2" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="I2" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="G2" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>35</v>
-      </c>
       <c r="J2" s="6" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="K2" s="8"/>
       <c r="L2" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="M2" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="M2" s="6" t="s">
-        <v>40</v>
+      <c r="N2" s="6" t="s">
+        <v>41</v>
       </c>
-      <c r="N2" s="6" t="s">
+      <c r="O2" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="O2" s="6" t="s">
-        <v>41</v>
-      </c>
       <c r="P2" s="7" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="Q2" s="8"/>
       <c r="R2" s="8"/>

</xml_diff>

<commit_message>
[HF-87][Zhenjia Zhou]fix: update excell template
</commit_message>
<xml_diff>
--- a/public/static/template/import_baby_en.xlsx
+++ b/public/static/template/import_baby_en.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhenjia.zhouthoughtworks.com/health-future-admin-frontend/public/static/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93260AEE-3753-CE43-B213-20A0FE89EF23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1469DE0E-32C8-4543-AC97-4DD3034F863B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="30580" windowHeight="19560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -141,11 +141,6 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">1.Required for EDC
-2.Due date should be after the current date.
-3.Format：YYYY-MM-DD </t>
-  </si>
-  <si>
     <t>1.Required for born babies.
 2.Birth day should be before the current date.
 3. Format：YYYY-MM-DD</t>
@@ -175,9 +170,18 @@
 Only allow 5-20 numbers.</t>
   </si>
   <si>
+    <t>1.Optional for born babies.
+2.Options：Add/No Add</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.Required
+2.Relatives Options: Mother/Father/Paternal Grandmother/Maternal Grandmother/Paternal Grandfather/Maternal Grandfather
+</t>
+  </si>
+  <si>
     <r>
       <t>1.Optional for born babies.
-2.Options：Exclusive Breastfeeding|| Formula Feeding || Mixed Breast/Formula Feeding || No Breast/Formula Feeding/</t>
+2.Options：Exclusive Breastfeeding||Formula Feeding || Mixed Breast/Formula Feeding || No Breast/Formula Feeding</t>
     </r>
     <r>
       <rPr>
@@ -191,38 +195,13 @@
     </r>
   </si>
   <si>
-    <r>
-      <t>1.Required
-2.Options:Born</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="12"/>
-        <rFont val="Monaco"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Monaco"/>
-        <family val="2"/>
-      </rPr>
-      <t>/Birth</t>
-    </r>
+    <t>1.Required
+2.Options:Unborn/Born</t>
   </si>
   <si>
-    <t>1.Optional for born babies.
-2.Options：Add/No Add</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.Required
-2.Relatives Options: Mother/Father/Paternal Grandmother/Maternal Grandmother/Paternal Grandfather/Maternal Grandfather
-</t>
+    <t xml:space="preserve">1.Required for Unborn
+2.Due date should be after the current date.
+3.Format：YYYY-MM-DD </t>
   </si>
 </sst>
 </file>
@@ -1482,8 +1461,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AC196"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13.75" customHeight="1"/>
@@ -1612,47 +1591,47 @@
         <v>28</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>29</v>
       </c>
       <c r="E2" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="G2" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="I2" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="G2" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>32</v>
-      </c>
       <c r="J2" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K2" s="8"/>
       <c r="L2" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M2" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="O2" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="N2" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="O2" s="6" t="s">
-        <v>37</v>
-      </c>
       <c r="P2" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="Q2" s="8"/>
       <c r="R2" s="8"/>

</xml_diff>

<commit_message>
[HF-87][Zhenjia Zhou]fix: update excel template
</commit_message>
<xml_diff>
--- a/public/static/template/import_baby_en.xlsx
+++ b/public/static/template/import_baby_en.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhenjia.zhouthoughtworks.com/health-future-admin-frontend/public/static/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1469DE0E-32C8-4543-AC97-4DD3034F863B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01A9E3A5-1BD0-F24A-83F3-53859C04108B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="30580" windowHeight="19560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -170,10 +170,6 @@
 Only allow 5-20 numbers.</t>
   </si>
   <si>
-    <t>1.Optional for born babies.
-2.Options：Add/No Add</t>
-  </si>
-  <si>
     <t xml:space="preserve">1.Required
 2.Relatives Options: Mother/Father/Paternal Grandmother/Maternal Grandmother/Paternal Grandfather/Maternal Grandfather
 </t>
@@ -202,6 +198,10 @@
     <t xml:space="preserve">1.Required for Unborn
 2.Due date should be after the current date.
 3.Format：YYYY-MM-DD </t>
+  </si>
+  <si>
+    <t>1.Optional for born babies.
+2.Options：Yes/No</t>
   </si>
 </sst>
 </file>
@@ -1461,8 +1461,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AC196"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13.75" customHeight="1"/>
@@ -1591,7 +1591,7 @@
         <v>28</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>34</v>
@@ -1600,16 +1600,16 @@
         <v>29</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F2" s="6" t="s">
         <v>30</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I2" s="6" t="s">
         <v>31</v>
@@ -1625,7 +1625,7 @@
         <v>35</v>
       </c>
       <c r="N2" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O2" s="6" t="s">
         <v>36</v>

</xml_diff>